<commit_message>
model updated and ready for Q2'25
</commit_message>
<xml_diff>
--- a/NVDA.xlsx
+++ b/NVDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameelbrannon/Library/CloudStorage/Dropbox/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B909E86B-DE91-9C49-8874-DBC356998655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288F70BA-9DF6-4D4E-B047-28D64E739AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19120" yWindow="500" windowWidth="48920" windowHeight="28280" activeTab="1" xr2:uid="{3991C303-FDF7-2343-B20E-E26B6CBB280D}"/>
+    <workbookView xWindow="57060" yWindow="500" windowWidth="48920" windowHeight="28280" xr2:uid="{3991C303-FDF7-2343-B20E-E26B6CBB280D}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="m/d;@"/>
-    <numFmt numFmtId="167" formatCode="0\x"/>
+    <numFmt numFmtId="165" formatCode="0\x"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -691,7 +691,7 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1160,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61C9843-BDE5-5E44-98C3-1A0D7B368C6B}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1201,7 +1201,7 @@
         <v>4</v>
       </c>
       <c r="K3" s="1">
-        <v>135.58000000000001</v>
+        <v>124.24</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1218,7 +1218,7 @@
         <v>24600</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M4" s="1">
         <f>+K4*10</f>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="K5" s="1">
         <f>+K3*K4</f>
-        <v>3335268.0000000005</v>
+        <v>3056304</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="L6" s="1" t="str">
         <f>+L4</f>
-        <v>Q125</v>
+        <v>Q225</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1263,7 +1263,7 @@
       </c>
       <c r="L7" s="1" t="str">
         <f>+L6</f>
-        <v>Q125</v>
+        <v>Q225</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="K8" s="1">
         <f>+K5-K6+K7</f>
-        <v>3318993.0000000005</v>
+        <v>3040029</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1421,11 +1421,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38A046E-F266-6848-AB04-142D610E732A}">
   <dimension ref="B2:ID87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AF8" sqref="AF8"/>
+      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1579,6 +1579,9 @@
       <c r="S3" s="7">
         <v>45410</v>
       </c>
+      <c r="T3" s="7">
+        <v>45350</v>
+      </c>
       <c r="Y3" s="7">
         <v>44227</v>
       </c>
@@ -5507,83 +5510,83 @@
         <v>35</v>
       </c>
       <c r="G37" s="3">
-        <f>+IFERROR(G13/C13-1,0)</f>
+        <f t="shared" ref="G37:V42" si="208">+IFERROR(G13/C13-1,0)</f>
         <v>0</v>
       </c>
       <c r="H37" s="3">
-        <f>+IFERROR(H13/D13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="I37" s="3">
-        <f>+IFERROR(I13/E13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="J37" s="3">
-        <f>+IFERROR(J13/F13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="K37" s="3">
-        <f>+IFERROR(K13/G13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>6.4039408866995107E-2</v>
       </c>
       <c r="L37" s="3">
-        <f>+IFERROR(L13/H13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="M37" s="3">
-        <f>+IFERROR(M13/I13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.26735303885752248</v>
       </c>
       <c r="N37" s="3">
-        <f>+IFERROR(N13/J13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>4.4254062038404722</v>
       </c>
       <c r="O37" s="3">
-        <f>+IFERROR(O13/K13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.21459694989106759</v>
       </c>
       <c r="P37" s="3">
-        <f>+IFERROR(P13/L13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>1.6624008190427437</v>
       </c>
       <c r="Q37" s="3">
-        <f>+IFERROR(Q13/M13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>2.8377882599580713</v>
       </c>
       <c r="R37" s="3">
-        <f>+IFERROR(R13/N13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>3.8728559760413832</v>
       </c>
       <c r="S37" s="3">
-        <f>+IFERROR(S13/O13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>4.0840807174887894</v>
       </c>
       <c r="T37" s="3">
-        <f>+IFERROR(T13/P13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>1.3435854387016235</v>
       </c>
       <c r="U37" s="3">
-        <f>+IFERROR(U13/Q13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.83105314487618442</v>
       </c>
       <c r="V37" s="3">
-        <f>+IFERROR(V13/R13-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.64808082676181122</v>
       </c>
       <c r="Z37" s="3">
-        <f>+Z13/Y13-1</f>
+        <f t="shared" ref="Z37:AC38" si="209">+Z13/Y13-1</f>
         <v>0.12324588163514338</v>
       </c>
       <c r="AA37" s="3">
-        <f>+AA13/Z13-1</f>
+        <f t="shared" si="209"/>
         <v>0.36411370631902962</v>
       </c>
       <c r="AB37" s="3">
-        <f>+AB13/AA13-1</f>
+        <f t="shared" si="209"/>
         <v>2.1460711441465357</v>
       </c>
       <c r="AC37" s="3">
-        <f>+AC13/AB13-1</f>
+        <f t="shared" si="209"/>
         <v>1.1804893930486005</v>
       </c>
       <c r="AQ37" s="26" t="s">
@@ -5599,83 +5602,83 @@
         <v>36</v>
       </c>
       <c r="G38" s="3">
-        <f>+IFERROR(G14/C14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="H38" s="3">
-        <f>+IFERROR(H14/D14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="I38" s="3">
-        <f>+IFERROR(I14/E14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="J38" s="3">
-        <f>+IFERROR(J14/F14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="K38" s="3">
-        <f>+IFERROR(K14/G14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>1.08868778280543</v>
       </c>
       <c r="L38" s="3">
-        <f>+IFERROR(L14/H14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>7.5769230769230811E-2</v>
       </c>
       <c r="M38" s="3">
-        <f>+IFERROR(M14/I14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>-0.48313782991202348</v>
       </c>
       <c r="N38" s="3">
-        <f>+IFERROR(N14/J14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>-0.65862761986792995</v>
       </c>
       <c r="O38" s="3">
-        <f>+IFERROR(O14/K14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>-0.40814558058925476</v>
       </c>
       <c r="P38" s="3">
-        <f>+IFERROR(P14/L14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.11011798355380775</v>
       </c>
       <c r="Q38" s="3">
-        <f>+IFERROR(Q14/M14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.64302600472813243</v>
       </c>
       <c r="R38" s="3">
-        <f>+IFERROR(R14/N14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.76829268292682928</v>
       </c>
       <c r="S38" s="3">
-        <f>+IFERROR(S14/O14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.23316251830161061</v>
       </c>
       <c r="T38" s="3">
-        <f>+IFERROR(T14/P14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.16651345140924656</v>
       </c>
       <c r="U38" s="3">
-        <f>+IFERROR(U14/Q14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.14654005562252714</v>
       </c>
       <c r="V38" s="3">
-        <f>+IFERROR(V14/R14-1,0)</f>
+        <f t="shared" si="208"/>
         <v>4.2247173036173757E-2</v>
       </c>
       <c r="Z38" s="3">
-        <f>+Z14/Y14-1</f>
+        <f t="shared" si="209"/>
         <v>1.3195439263265603</v>
       </c>
       <c r="AA38" s="3">
-        <f>+AA14/Z14-1</f>
+        <f t="shared" si="209"/>
         <v>-0.24968490042853542</v>
       </c>
       <c r="AB38" s="3">
-        <f>+AB14/AA14-1</f>
+        <f t="shared" si="209"/>
         <v>0.13530992776751227</v>
       </c>
       <c r="AC38" s="3">
-        <f>+AC14/AB14-1</f>
+        <f t="shared" si="209"/>
         <v>0.13619148646379386</v>
       </c>
       <c r="AQ38" s="11" t="s">
@@ -5683,7 +5686,7 @@
       </c>
       <c r="AR38" s="12">
         <f>+Main!K3</f>
-        <v>135.58000000000001</v>
+        <v>124.24</v>
       </c>
     </row>
     <row r="39" spans="2:44" s="20" customFormat="1">
@@ -5691,122 +5694,122 @@
         <v>20</v>
       </c>
       <c r="G39" s="20">
-        <f>+IFERROR(G15/C15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="H39" s="20">
-        <f>+IFERROR(H15/D15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="I39" s="20">
-        <f>+IFERROR(I15/E15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="J39" s="20">
-        <f>+IFERROR(J15/F15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="K39" s="20">
-        <f>+IFERROR(K15/G15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.46405228758169925</v>
       </c>
       <c r="L39" s="20">
-        <f>+IFERROR(L15/H15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>3.0275088366374714E-2</v>
       </c>
       <c r="M39" s="20">
-        <f>+IFERROR(M15/I15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>-0.16500070392791777</v>
       </c>
       <c r="N39" s="20">
-        <f>+IFERROR(N15/J15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>-0.20829517205285886</v>
       </c>
       <c r="O39" s="20">
-        <f>+IFERROR(O15/K15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>-0.13223938223938225</v>
       </c>
       <c r="P39" s="20">
-        <f>+IFERROR(P15/L15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>1.0147673031026252</v>
       </c>
       <c r="Q39" s="20">
-        <f>+IFERROR(Q15/M15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>2.0551340414769852</v>
       </c>
       <c r="R39" s="20">
-        <f>+IFERROR(R15/N15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>2.6527846636919516</v>
       </c>
       <c r="S39" s="20">
-        <f>+IFERROR(S15/O15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>2.6212458286985538</v>
       </c>
       <c r="T39" s="20">
-        <f>+IFERROR(T15/P15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>1.072999185607463</v>
       </c>
       <c r="U39" s="20">
-        <f>+IFERROR(U15/Q15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.69977924944812386</v>
       </c>
       <c r="V39" s="20">
-        <f>+IFERROR(V15/R15-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.5328235986065244</v>
       </c>
       <c r="Y39" s="20">
-        <f>+Y15/X15-1</f>
+        <f t="shared" ref="Y39:Z42" si="210">+Y15/X15-1</f>
         <v>0.52729437625938824</v>
       </c>
       <c r="Z39" s="20">
-        <f>+Z15/Y15-1</f>
+        <f t="shared" si="210"/>
         <v>0.61403298350824587</v>
       </c>
       <c r="AA39" s="20">
         <v>0</v>
       </c>
       <c r="AB39" s="20">
-        <f>+AB15/AA15-1</f>
+        <f t="shared" ref="AB39:AL39" si="211">+AB15/AA15-1</f>
         <v>1.2585452658115224</v>
       </c>
       <c r="AC39" s="20">
-        <f>+AC15/AB15-1</f>
+        <f t="shared" si="211"/>
         <v>0.9487869735071075</v>
       </c>
       <c r="AD39" s="20">
-        <f>+AD15/AC15-1</f>
+        <f t="shared" si="211"/>
         <v>0.39999999999999991</v>
       </c>
       <c r="AE39" s="20">
-        <f>+AE15/AD15-1</f>
+        <f t="shared" si="211"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="AF39" s="20">
-        <f>+AF15/AE15-1</f>
+        <f t="shared" si="211"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AG39" s="20">
-        <f>+AG15/AF15-1</f>
+        <f t="shared" si="211"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AH39" s="20">
-        <f>+AH15/AG15-1</f>
+        <f t="shared" si="211"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AI39" s="20">
-        <f>+AI15/AH15-1</f>
+        <f t="shared" si="211"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AJ39" s="20">
-        <f>+AJ15/AI15-1</f>
+        <f t="shared" si="211"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AK39" s="20">
-        <f>+AK15/AJ15-1</f>
+        <f t="shared" si="211"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AL39" s="20">
-        <f>+AL15/AK15-1</f>
+        <f t="shared" si="211"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AQ39" s="32" t="s">
@@ -5814,7 +5817,7 @@
       </c>
       <c r="AR39" s="33">
         <f>+AR37/AR38-1</f>
-        <v>2.7238990235035176E-2</v>
+        <v>0.12100017945964336</v>
       </c>
     </row>
     <row r="40" spans="2:44" s="3" customFormat="1">
@@ -5822,75 +5825,75 @@
         <v>21</v>
       </c>
       <c r="G40" s="3">
-        <f>+IFERROR(G16/C16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="H40" s="3">
-        <f>+IFERROR(H16/D16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="I40" s="3">
-        <f>+IFERROR(I16/E16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="J40" s="3">
-        <f>+IFERROR(J16/F16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="K40" s="3">
-        <f>+IFERROR(K16/G16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.40600393700787407</v>
       </c>
       <c r="L40" s="3">
-        <f>+IFERROR(L16/H16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.65314136125654443</v>
       </c>
       <c r="M40" s="3">
-        <f>+IFERROR(M16/I16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.11407766990291268</v>
       </c>
       <c r="N40" s="3">
-        <f>+IFERROR(N16/J16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>-0.16080211880438899</v>
       </c>
       <c r="O40" s="3">
-        <f>+IFERROR(O16/K16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>-0.10955547777388874</v>
       </c>
       <c r="P40" s="3">
-        <f>+IFERROR(P16/L16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>6.7564001055687495E-2</v>
       </c>
       <c r="Q40" s="3">
-        <f>+IFERROR(Q16/M16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.71387073347857655</v>
       </c>
       <c r="R40" s="3">
-        <f>+IFERROR(R16/N16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>1.394950405770965</v>
       </c>
       <c r="S40" s="3">
-        <f>+IFERROR(S16/O16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>1.216194968553459</v>
       </c>
       <c r="T40" s="3">
-        <f>+IFERROR(T16/P16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>1.0729991856074625</v>
       </c>
       <c r="U40" s="3">
-        <f>+IFERROR(U16/Q16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.69977924944812386</v>
       </c>
       <c r="V40" s="3">
-        <f>+IFERROR(V16/R16-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.5328235986065244</v>
       </c>
       <c r="Y40" s="3">
-        <f>+Y16/X16-1</f>
+        <f t="shared" si="210"/>
         <v>0.51301204819277113</v>
       </c>
       <c r="Z40" s="3">
-        <f>+Z16/Y16-1</f>
+        <f t="shared" si="210"/>
         <v>0.5032648510909381</v>
       </c>
       <c r="AA40" s="3">
@@ -5898,47 +5901,47 @@
         <v>0.23085072571246945</v>
       </c>
       <c r="AB40" s="3">
-        <f>+AB16/AA16-1</f>
+        <f t="shared" ref="AB40:AL40" si="212">+AB16/AA16-1</f>
         <v>0.43062489240833179</v>
       </c>
       <c r="AC40" s="3">
-        <f>+AC16/AB16-1</f>
+        <f t="shared" si="212"/>
         <v>0.81629256476597023</v>
       </c>
       <c r="AD40" s="3">
-        <f>+AD16/AC16-1</f>
+        <f t="shared" si="212"/>
         <v>0.39999999999999969</v>
       </c>
       <c r="AE40" s="3">
-        <f>+AE16/AD16-1</f>
+        <f t="shared" si="212"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="AF40" s="3">
-        <f>+AF16/AE16-1</f>
+        <f t="shared" si="212"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AG40" s="3">
-        <f>+AG16/AF16-1</f>
+        <f t="shared" si="212"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="AH40" s="3">
-        <f>+AH16/AG16-1</f>
+        <f t="shared" si="212"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AI40" s="3">
-        <f>+AI16/AH16-1</f>
+        <f t="shared" si="212"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AJ40" s="3">
-        <f>+AJ16/AI16-1</f>
+        <f t="shared" si="212"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="AK40" s="3">
-        <f>+AK16/AJ16-1</f>
+        <f t="shared" si="212"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AL40" s="3">
-        <f>+AL16/AK16-1</f>
+        <f t="shared" si="212"/>
         <v>0.19999999999999996</v>
       </c>
     </row>
@@ -5947,75 +5950,75 @@
         <v>22</v>
       </c>
       <c r="G41" s="3">
-        <f>+IFERROR(G17/C17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="H41" s="3">
-        <f>+IFERROR(H17/D17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="I41" s="3">
-        <f>+IFERROR(I17/E17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="J41" s="3">
-        <f>+IFERROR(J17/F17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="K41" s="3">
-        <f>+IFERROR(K17/G17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.40329575021682573</v>
       </c>
       <c r="L41" s="3">
-        <f>+IFERROR(L17/H17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.46506024096385534</v>
       </c>
       <c r="M41" s="3">
-        <f>+IFERROR(M17/I17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.38631503920171073</v>
       </c>
       <c r="N41" s="3">
-        <f>+IFERROR(N17/J17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.3306066802999319</v>
       </c>
       <c r="O41" s="3">
-        <f>+IFERROR(O17/K17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.15883807169344877</v>
       </c>
       <c r="P41" s="3">
-        <f>+IFERROR(P17/L17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.11842105263157898</v>
       </c>
       <c r="Q41" s="3">
-        <f>+IFERROR(Q17/M17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.17943444730077118</v>
       </c>
       <c r="R41" s="3">
-        <f>+IFERROR(R17/N17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.26331967213114749</v>
       </c>
       <c r="S41" s="3">
-        <f>+IFERROR(S17/O17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.45066666666666677</v>
       </c>
       <c r="T41" s="3">
-        <f>+IFERROR(T17/P17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.47058823529411775</v>
       </c>
       <c r="U41" s="3">
-        <f>+IFERROR(U17/Q17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.69977924944812386</v>
       </c>
       <c r="V41" s="3">
-        <f>+IFERROR(V17/R17-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.5328235986065244</v>
       </c>
       <c r="Y41" s="3">
-        <f>+Y17/X17-1</f>
+        <f t="shared" si="210"/>
         <v>0.38706256627783664</v>
       </c>
       <c r="Z41" s="3">
-        <f>+Z17/Y17-1</f>
+        <f t="shared" si="210"/>
         <v>0.34250764525993893</v>
       </c>
       <c r="AA41" s="3">
@@ -6023,47 +6026,47 @@
         <v>0.39312832194381175</v>
       </c>
       <c r="AB41" s="3">
-        <f>+AB17/AA17-1</f>
+        <f t="shared" ref="AB41:AL41" si="213">+AB17/AA17-1</f>
         <v>0.18204115002043886</v>
       </c>
       <c r="AC41" s="3">
-        <f>+AC17/AB17-1</f>
+        <f t="shared" si="213"/>
         <v>0.54458058701990586</v>
       </c>
       <c r="AD41" s="3">
-        <f>+AD17/AC17-1</f>
+        <f t="shared" si="213"/>
         <v>0.39999999999999969</v>
       </c>
       <c r="AE41" s="3">
-        <f>+AE17/AD17-1</f>
+        <f t="shared" si="213"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="AF41" s="3">
-        <f>+AF17/AE17-1</f>
+        <f t="shared" si="213"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="AG41" s="3">
-        <f>+AG17/AF17-1</f>
+        <f t="shared" si="213"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AH41" s="3">
-        <f>+AH17/AG17-1</f>
+        <f t="shared" si="213"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AI41" s="3">
-        <f>+AI17/AH17-1</f>
+        <f t="shared" si="213"/>
         <v>0.19999999999999973</v>
       </c>
       <c r="AJ41" s="3">
-        <f>+AJ17/AI17-1</f>
+        <f t="shared" si="213"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AK41" s="3">
-        <f>+AK17/AJ17-1</f>
+        <f t="shared" si="213"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="AL41" s="3">
-        <f>+AL17/AK17-1</f>
+        <f t="shared" si="213"/>
         <v>0.19999999999999996</v>
       </c>
     </row>
@@ -6072,75 +6075,75 @@
         <v>23</v>
       </c>
       <c r="G42" s="3">
-        <f>+IFERROR(G18/C18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="H42" s="3">
-        <f>+IFERROR(H18/D18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="I42" s="3">
-        <f>+IFERROR(I18/E18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="J42" s="3">
-        <f>+IFERROR(J18/F18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0</v>
       </c>
       <c r="K42" s="3">
-        <f>+IFERROR(K18/G18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.13846153846153841</v>
       </c>
       <c r="L42" s="3">
-        <f>+IFERROR(L18/H18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.12547528517110274</v>
       </c>
       <c r="M42" s="3">
-        <f>+IFERROR(M18/I18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.1328545780969479</v>
       </c>
       <c r="N42" s="3">
-        <f>+IFERROR(N18/J18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.11012433392539966</v>
       </c>
       <c r="O42" s="3">
-        <f>+IFERROR(O18/K18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>6.9256756756756799E-2</v>
       </c>
       <c r="P42" s="3">
-        <f>+IFERROR(P18/L18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>5.0675675675675658E-2</v>
       </c>
       <c r="Q42" s="3">
-        <f>+IFERROR(Q18/M18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>9.191759112519815E-2</v>
       </c>
       <c r="R42" s="3">
-        <f>+IFERROR(R18/N18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.1359999999999999</v>
       </c>
       <c r="S42" s="3">
-        <f>+IFERROR(S18/O18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.22748815165876768</v>
       </c>
       <c r="T42" s="3">
-        <f>+IFERROR(T18/P18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.60771704180064301</v>
       </c>
       <c r="U42" s="3">
-        <f>+IFERROR(U18/Q18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.69977924944812409</v>
       </c>
       <c r="V42" s="3">
-        <f>+IFERROR(V18/R18-1,0)</f>
+        <f t="shared" si="208"/>
         <v>0.5328235986065244</v>
       </c>
       <c r="Y42" s="3">
-        <f>+Y18/X18-1</f>
+        <f t="shared" si="210"/>
         <v>0.77493138151875574</v>
       </c>
       <c r="Z42" s="3">
-        <f>+Z18/Y18-1</f>
+        <f t="shared" si="210"/>
         <v>0.11649484536082477</v>
       </c>
       <c r="AA42" s="3">
@@ -6148,47 +6151,47 @@
         <v>0.12650046168051698</v>
       </c>
       <c r="AB42" s="3">
-        <f>+AB18/AA18-1</f>
+        <f t="shared" ref="AB42:AL42" si="214">+AB18/AA18-1</f>
         <v>8.7704918032786905E-2</v>
       </c>
       <c r="AC42" s="3">
-        <f>+AC18/AB18-1</f>
+        <f t="shared" si="214"/>
         <v>0.52089399317271656</v>
       </c>
       <c r="AD42" s="3">
-        <f>+AD18/AC18-1</f>
+        <f t="shared" si="214"/>
         <v>0.39999999999999969</v>
       </c>
       <c r="AE42" s="3">
-        <f>+AE18/AD18-1</f>
+        <f t="shared" si="214"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="AF42" s="3">
-        <f>+AF18/AE18-1</f>
+        <f t="shared" si="214"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AG42" s="3">
-        <f>+AG18/AF18-1</f>
+        <f t="shared" si="214"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AH42" s="3">
-        <f>+AH18/AG18-1</f>
+        <f t="shared" si="214"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AI42" s="3">
-        <f>+AI18/AH18-1</f>
+        <f t="shared" si="214"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AJ42" s="3">
-        <f>+AJ18/AI18-1</f>
+        <f t="shared" si="214"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AK42" s="3">
-        <f>+AK18/AJ18-1</f>
+        <f t="shared" si="214"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="AL42" s="3">
-        <f>+AL18/AK18-1</f>
+        <f t="shared" si="214"/>
         <v>0.19999999999999996</v>
       </c>
     </row>
@@ -6198,60 +6201,60 @@
       </c>
       <c r="AR43" s="22">
         <f>+Main!$K$8/Model!AC26</f>
-        <v>54.460141567687693</v>
+        <v>49.882723377203874</v>
       </c>
     </row>
     <row r="44" spans="2:44" s="3" customFormat="1">
       <c r="Z44" s="3">
-        <f>+Z16/Z$15</f>
+        <f t="shared" ref="Z44:AL44" si="215">+Z16/Z$15</f>
         <v>0.35070966783086871</v>
       </c>
       <c r="AA44" s="3">
-        <f>+AA16/AA$15</f>
+        <f t="shared" si="215"/>
         <v>0.43071105509008673</v>
       </c>
       <c r="AB44" s="3">
-        <f>+AB16/AB$15</f>
+        <f t="shared" si="215"/>
         <v>0.27282426709563046</v>
       </c>
       <c r="AC44" s="3">
-        <f>+AC16/AC$15</f>
+        <f t="shared" si="215"/>
         <v>0.2542754516270947</v>
       </c>
       <c r="AD44" s="3">
-        <f>+AD16/AD$15</f>
+        <f t="shared" si="215"/>
         <v>0.2542754516270947</v>
       </c>
       <c r="AE44" s="3">
-        <f>+AE16/AE$15</f>
+        <f t="shared" si="215"/>
         <v>0.2542754516270947</v>
       </c>
       <c r="AF44" s="3">
-        <f>+AF16/AF$15</f>
+        <f t="shared" si="215"/>
         <v>0.2542754516270947</v>
       </c>
       <c r="AG44" s="3">
-        <f>+AG16/AG$15</f>
+        <f t="shared" si="215"/>
         <v>0.2542754516270947</v>
       </c>
       <c r="AH44" s="3">
-        <f>+AH16/AH$15</f>
+        <f t="shared" si="215"/>
         <v>0.2542754516270947</v>
       </c>
       <c r="AI44" s="3">
-        <f>+AI16/AI$15</f>
+        <f t="shared" si="215"/>
         <v>0.2542754516270947</v>
       </c>
       <c r="AJ44" s="3">
-        <f>+AJ16/AJ$15</f>
+        <f t="shared" si="215"/>
         <v>0.2542754516270947</v>
       </c>
       <c r="AK44" s="3">
-        <f>+AK16/AK$15</f>
+        <f t="shared" si="215"/>
         <v>0.2542754516270947</v>
       </c>
       <c r="AL44" s="3">
-        <f>+AL16/AL$15</f>
+        <f t="shared" si="215"/>
         <v>0.2542754516270947</v>
       </c>
       <c r="AQ44" s="1" t="s">
@@ -6259,60 +6262,60 @@
       </c>
       <c r="AR44" s="22">
         <f>+Main!$K$8/Model!AD26</f>
-        <v>39.654751676344397</v>
+        <v>36.321738275400271</v>
       </c>
     </row>
     <row r="45" spans="2:44" s="3" customFormat="1">
       <c r="Z45" s="3">
-        <f>+Z17/Z$15</f>
+        <f t="shared" ref="Z45:AL45" si="216">+Z17/Z$15</f>
         <v>0.19573456193802483</v>
       </c>
       <c r="AA45" s="3">
-        <f>+AA17/AA$15</f>
+        <f t="shared" si="216"/>
         <v>0.27207681471046191</v>
       </c>
       <c r="AB45" s="3">
-        <f>+AB17/AB$15</f>
+        <f t="shared" si="216"/>
         <v>0.14239519385443683</v>
       </c>
       <c r="AC45" s="3">
-        <f>+AC17/AC$15</f>
+        <f t="shared" si="216"/>
         <v>0.11286038705230352</v>
       </c>
       <c r="AD45" s="3">
-        <f>+AD17/AD$15</f>
+        <f t="shared" si="216"/>
         <v>0.11286038705230352</v>
       </c>
       <c r="AE45" s="3">
-        <f>+AE17/AE$15</f>
+        <f t="shared" si="216"/>
         <v>0.11286038705230352</v>
       </c>
       <c r="AF45" s="3">
-        <f>+AF17/AF$15</f>
+        <f t="shared" si="216"/>
         <v>0.11286038705230352</v>
       </c>
       <c r="AG45" s="3">
-        <f>+AG17/AG$15</f>
+        <f t="shared" si="216"/>
         <v>0.11286038705230353</v>
       </c>
       <c r="AH45" s="3">
-        <f>+AH17/AH$15</f>
+        <f t="shared" si="216"/>
         <v>0.11286038705230352</v>
       </c>
       <c r="AI45" s="3">
-        <f>+AI17/AI$15</f>
+        <f t="shared" si="216"/>
         <v>0.11286038705230352</v>
       </c>
       <c r="AJ45" s="3">
-        <f>+AJ17/AJ$15</f>
+        <f t="shared" si="216"/>
         <v>0.11286038705230352</v>
       </c>
       <c r="AK45" s="3">
-        <f>+AK17/AK$15</f>
+        <f t="shared" si="216"/>
         <v>0.11286038705230353</v>
       </c>
       <c r="AL45" s="3">
-        <f>+AL17/AL$15</f>
+        <f t="shared" si="216"/>
         <v>0.11286038705230353</v>
       </c>
       <c r="AQ45" s="1" t="s">
@@ -6324,55 +6327,55 @@
     </row>
     <row r="46" spans="2:44" s="3" customFormat="1">
       <c r="Z46" s="3">
-        <f>+Z18/Z$15</f>
+        <f t="shared" ref="Z46:AL46" si="217">+Z18/Z$15</f>
         <v>8.0478561343538674E-2</v>
       </c>
       <c r="AA46" s="3">
-        <f>+AA18/AA$15</f>
+        <f t="shared" si="217"/>
         <v>9.0457477570994288E-2</v>
       </c>
       <c r="AB46" s="3">
-        <f>+AB18/AB$15</f>
+        <f t="shared" si="217"/>
         <v>4.3563901382095135E-2</v>
       </c>
       <c r="AC46" s="3">
-        <f>+AC18/AC$15</f>
+        <f t="shared" si="217"/>
         <v>3.3998624186182991E-2</v>
       </c>
       <c r="AD46" s="3">
-        <f>+AD18/AD$15</f>
+        <f t="shared" si="217"/>
         <v>3.3998624186182991E-2</v>
       </c>
       <c r="AE46" s="3">
-        <f>+AE18/AE$15</f>
+        <f t="shared" si="217"/>
         <v>3.3998624186182991E-2</v>
       </c>
       <c r="AF46" s="3">
-        <f>+AF18/AF$15</f>
+        <f t="shared" si="217"/>
         <v>3.3998624186182991E-2</v>
       </c>
       <c r="AG46" s="3">
-        <f>+AG18/AG$15</f>
+        <f t="shared" si="217"/>
         <v>3.3998624186182991E-2</v>
       </c>
       <c r="AH46" s="3">
-        <f>+AH18/AH$15</f>
+        <f t="shared" si="217"/>
         <v>3.3998624186182991E-2</v>
       </c>
       <c r="AI46" s="3">
-        <f>+AI18/AI$15</f>
+        <f t="shared" si="217"/>
         <v>3.3998624186182991E-2</v>
       </c>
       <c r="AJ46" s="3">
-        <f>+AJ18/AJ$15</f>
+        <f t="shared" si="217"/>
         <v>3.3998624186182991E-2</v>
       </c>
       <c r="AK46" s="3">
-        <f>+AK18/AK$15</f>
+        <f t="shared" si="217"/>
         <v>3.3998624186182991E-2</v>
       </c>
       <c r="AL46" s="3">
-        <f>+AL18/AL$15</f>
+        <f t="shared" si="217"/>
         <v>3.3998624186182991E-2</v>
       </c>
     </row>
@@ -6381,47 +6384,47 @@
         <v>84</v>
       </c>
       <c r="F49" s="4">
-        <f t="shared" ref="F49:P49" si="208">SUM(F50:F51)-SUM(F66,F68)</f>
+        <f t="shared" ref="F49:P49" si="218">SUM(F50:F51)-SUM(F66,F68)</f>
         <v>0</v>
       </c>
       <c r="G49" s="4">
-        <f t="shared" si="208"/>
+        <f t="shared" si="218"/>
         <v>0</v>
       </c>
       <c r="H49" s="4">
-        <f t="shared" si="208"/>
+        <f t="shared" si="218"/>
         <v>0</v>
       </c>
       <c r="I49" s="4">
-        <f t="shared" si="208"/>
+        <f t="shared" si="218"/>
         <v>0</v>
       </c>
       <c r="J49" s="4">
-        <f t="shared" si="208"/>
+        <f t="shared" si="218"/>
         <v>0</v>
       </c>
       <c r="K49" s="4">
-        <f t="shared" si="208"/>
+        <f t="shared" si="218"/>
         <v>0</v>
       </c>
       <c r="L49" s="4">
-        <f t="shared" si="208"/>
+        <f t="shared" si="218"/>
         <v>6088</v>
       </c>
       <c r="M49" s="4">
-        <f t="shared" si="208"/>
+        <f t="shared" si="218"/>
         <v>2193</v>
       </c>
       <c r="N49" s="4">
-        <f t="shared" si="208"/>
+        <f t="shared" si="218"/>
         <v>2343</v>
       </c>
       <c r="O49" s="4">
-        <f t="shared" si="208"/>
+        <f t="shared" si="218"/>
         <v>4366</v>
       </c>
       <c r="P49" s="4">
-        <f t="shared" si="208"/>
+        <f t="shared" si="218"/>
         <v>6318</v>
       </c>
       <c r="Q49" s="4">
@@ -6445,39 +6448,39 @@
         <v>22162.560000000001</v>
       </c>
       <c r="AD49" s="4">
-        <f t="shared" ref="AD49:AL49" si="209">+AC49*1.02</f>
+        <f t="shared" ref="AD49:AL49" si="219">+AC49*1.02</f>
         <v>22605.8112</v>
       </c>
       <c r="AE49" s="4">
-        <f t="shared" si="209"/>
+        <f t="shared" si="219"/>
         <v>23057.927424000001</v>
       </c>
       <c r="AF49" s="4">
-        <f t="shared" si="209"/>
+        <f t="shared" si="219"/>
         <v>23519.085972480003</v>
       </c>
       <c r="AG49" s="4">
-        <f t="shared" si="209"/>
+        <f t="shared" si="219"/>
         <v>23989.467691929603</v>
       </c>
       <c r="AH49" s="4">
-        <f t="shared" si="209"/>
+        <f t="shared" si="219"/>
         <v>24469.257045768198</v>
       </c>
       <c r="AI49" s="4">
-        <f t="shared" si="209"/>
+        <f t="shared" si="219"/>
         <v>24958.642186683563</v>
       </c>
       <c r="AJ49" s="4">
-        <f t="shared" si="209"/>
+        <f t="shared" si="219"/>
         <v>25457.815030417234</v>
       </c>
       <c r="AK49" s="4">
-        <f t="shared" si="209"/>
+        <f t="shared" si="219"/>
         <v>25966.971331025579</v>
       </c>
       <c r="AL49" s="4">
-        <f t="shared" si="209"/>
+        <f t="shared" si="219"/>
         <v>26486.31075764609</v>
       </c>
     </row>
@@ -6631,35 +6634,35 @@
         <v>68</v>
       </c>
       <c r="L55" s="1">
-        <f>+SUM(L50:L54)</f>
+        <f t="shared" ref="L55:S55" si="220">+SUM(L50:L54)</f>
         <v>27418</v>
       </c>
       <c r="M55" s="1">
-        <f>+SUM(M50:M54)</f>
+        <f t="shared" si="220"/>
         <v>23223</v>
       </c>
       <c r="N55" s="1">
-        <f>+SUM(N50:N54)</f>
+        <f t="shared" si="220"/>
         <v>23073</v>
       </c>
       <c r="O55" s="1">
-        <f>+SUM(O50:O54)</f>
+        <f t="shared" si="220"/>
         <v>24883</v>
       </c>
       <c r="P55" s="1">
-        <f>+SUM(P50:P54)</f>
+        <f t="shared" si="220"/>
         <v>28797</v>
       </c>
       <c r="Q55" s="1">
-        <f>+SUM(Q50:Q54)</f>
+        <f t="shared" si="220"/>
         <v>32658</v>
       </c>
       <c r="R55" s="1">
-        <f>+SUM(R50:R54)</f>
+        <f t="shared" si="220"/>
         <v>44345</v>
       </c>
       <c r="S55" s="1">
-        <f>+SUM(S50:S54)</f>
+        <f t="shared" si="220"/>
         <v>53729</v>
       </c>
     </row>
@@ -6842,35 +6845,35 @@
         <v>75</v>
       </c>
       <c r="L62" s="4">
-        <f>+SUM(L55:L61)</f>
+        <f t="shared" ref="L62:S62" si="221">+SUM(L55:L61)</f>
         <v>43476</v>
       </c>
       <c r="M62" s="4">
-        <f>+SUM(M55:M61)</f>
+        <f t="shared" si="221"/>
         <v>40488</v>
       </c>
       <c r="N62" s="4">
-        <f>+SUM(N55:N61)</f>
+        <f t="shared" si="221"/>
         <v>41182</v>
       </c>
       <c r="O62" s="4">
-        <f>+SUM(O55:O61)</f>
+        <f t="shared" si="221"/>
         <v>44460</v>
       </c>
       <c r="P62" s="4">
-        <f>+SUM(P55:P61)</f>
+        <f t="shared" si="221"/>
         <v>49555</v>
       </c>
       <c r="Q62" s="4">
-        <f>+SUM(Q55:Q61)</f>
+        <f t="shared" si="221"/>
         <v>54148</v>
       </c>
       <c r="R62" s="4">
-        <f>+SUM(R55:R61)</f>
+        <f t="shared" si="221"/>
         <v>65728</v>
       </c>
       <c r="S62" s="4">
-        <f>+SUM(S55:S61)</f>
+        <f t="shared" si="221"/>
         <v>77072</v>
       </c>
     </row>
@@ -6966,35 +6969,35 @@
         <v>80</v>
       </c>
       <c r="L67" s="1">
-        <f>+SUM(L64:L66)</f>
+        <f t="shared" ref="L67:S67" si="222">+SUM(L64:L66)</f>
         <v>7573</v>
       </c>
       <c r="M67" s="1">
-        <f>+SUM(M64:M66)</f>
+        <f t="shared" si="222"/>
         <v>6855</v>
       </c>
       <c r="N67" s="1">
-        <f>+SUM(N64:N66)</f>
+        <f t="shared" si="222"/>
         <v>6563</v>
       </c>
       <c r="O67" s="1">
-        <f>+SUM(O64:O66)</f>
+        <f t="shared" si="222"/>
         <v>7260</v>
       </c>
       <c r="P67" s="1">
-        <f>+SUM(P64:P66)</f>
+        <f t="shared" si="222"/>
         <v>10334</v>
       </c>
       <c r="Q67" s="1">
-        <f>+SUM(Q64:Q66)</f>
+        <f t="shared" si="222"/>
         <v>9101</v>
       </c>
       <c r="R67" s="1">
-        <f>+SUM(R64:R66)</f>
+        <f t="shared" si="222"/>
         <v>10631</v>
       </c>
       <c r="S67" s="1">
-        <f>+SUM(S64:S66)</f>
+        <f t="shared" si="222"/>
         <v>15223</v>
       </c>
     </row>
@@ -7090,35 +7093,35 @@
         <v>76</v>
       </c>
       <c r="L71" s="4">
-        <f>+SUM(L67:L70)</f>
+        <f t="shared" ref="L71:S71" si="223">+SUM(L67:L70)</f>
         <v>19625</v>
       </c>
       <c r="M71" s="4">
-        <f>+SUM(M67:M70)</f>
+        <f t="shared" si="223"/>
         <v>19139</v>
       </c>
       <c r="N71" s="4">
-        <f>+SUM(N67:N70)</f>
+        <f t="shared" si="223"/>
         <v>19081</v>
       </c>
       <c r="O71" s="4">
-        <f>+SUM(O67:O70)</f>
+        <f t="shared" si="223"/>
         <v>19940</v>
       </c>
       <c r="P71" s="4">
-        <f>+SUM(P67:P70)</f>
+        <f t="shared" si="223"/>
         <v>22054</v>
       </c>
       <c r="Q71" s="4">
-        <f>+SUM(Q67:Q70)</f>
+        <f t="shared" si="223"/>
         <v>20883</v>
       </c>
       <c r="R71" s="4">
-        <f>+SUM(R67:R70)</f>
+        <f t="shared" si="223"/>
         <v>22750</v>
       </c>
       <c r="S71" s="4">
-        <f>+SUM(S67:S70)</f>
+        <f t="shared" si="223"/>
         <v>27930</v>
       </c>
     </row>
@@ -7156,77 +7159,77 @@
         <v>104</v>
       </c>
       <c r="L73" s="4">
-        <f>+SUM(L71:L72)</f>
+        <f t="shared" ref="L73:S73" si="224">+SUM(L71:L72)</f>
         <v>43476</v>
       </c>
       <c r="M73" s="4">
-        <f>+SUM(M71:M72)</f>
+        <f t="shared" si="224"/>
         <v>40488</v>
       </c>
       <c r="N73" s="4">
-        <f>+SUM(N71:N72)</f>
+        <f t="shared" si="224"/>
         <v>41182</v>
       </c>
       <c r="O73" s="4">
-        <f>+SUM(O71:O72)</f>
+        <f t="shared" si="224"/>
         <v>44460</v>
       </c>
       <c r="P73" s="4">
-        <f>+SUM(P71:P72)</f>
+        <f t="shared" si="224"/>
         <v>49555</v>
       </c>
       <c r="Q73" s="4">
-        <f>+SUM(Q71:Q72)</f>
+        <f t="shared" si="224"/>
         <v>54148</v>
       </c>
       <c r="R73" s="4">
-        <f>+SUM(R71:R72)</f>
+        <f t="shared" si="224"/>
         <v>65728</v>
       </c>
       <c r="S73" s="4">
-        <f>+SUM(S71:S72)</f>
+        <f t="shared" si="224"/>
         <v>77072</v>
       </c>
     </row>
     <row r="74" spans="2:19">
       <c r="I74" s="4" t="str">
-        <f t="shared" ref="I74:R74" si="210">IF(I73=I62,"","DUQWDGWTDGWD")</f>
+        <f t="shared" ref="I74:R74" si="225">IF(I73=I62,"","DUQWDGWTDGWD")</f>
         <v/>
       </c>
       <c r="J74" s="4" t="str">
-        <f t="shared" si="210"/>
+        <f t="shared" si="225"/>
         <v/>
       </c>
       <c r="K74" s="4" t="str">
-        <f t="shared" si="210"/>
+        <f t="shared" si="225"/>
         <v/>
       </c>
       <c r="L74" s="4" t="str">
-        <f t="shared" si="210"/>
+        <f t="shared" si="225"/>
         <v/>
       </c>
       <c r="M74" s="4" t="str">
-        <f t="shared" si="210"/>
+        <f t="shared" si="225"/>
         <v/>
       </c>
       <c r="N74" s="4" t="str">
-        <f t="shared" si="210"/>
+        <f t="shared" si="225"/>
         <v/>
       </c>
       <c r="O74" s="4" t="str">
-        <f t="shared" si="210"/>
+        <f t="shared" si="225"/>
         <v/>
       </c>
       <c r="P74" s="4" t="str">
-        <f t="shared" si="210"/>
+        <f t="shared" si="225"/>
         <v/>
       </c>
       <c r="Q74" s="4" t="str">
-        <f t="shared" si="210"/>
+        <f t="shared" si="225"/>
         <v/>
       </c>
       <c r="R74" s="4" t="str">
-        <f t="shared" si="210"/>
+        <f t="shared" si="225"/>
         <v/>
       </c>
       <c r="S74" s="4" t="str">
@@ -7243,31 +7246,31 @@
         <v>17037</v>
       </c>
       <c r="M75" s="1">
-        <f t="shared" ref="M75:S75" si="211">+SUM(M50:M51)</f>
+        <f t="shared" ref="M75:S75" si="226">+SUM(M50:M51)</f>
         <v>13143</v>
       </c>
       <c r="N75" s="1">
-        <f t="shared" si="211"/>
+        <f t="shared" si="226"/>
         <v>13296</v>
       </c>
       <c r="O75" s="1">
-        <f t="shared" si="211"/>
+        <f t="shared" si="226"/>
         <v>15320</v>
       </c>
       <c r="P75" s="1">
-        <f t="shared" si="211"/>
+        <f t="shared" si="226"/>
         <v>16023</v>
       </c>
       <c r="Q75" s="1">
-        <f t="shared" si="211"/>
+        <f t="shared" si="226"/>
         <v>18281</v>
       </c>
       <c r="R75" s="1">
-        <f t="shared" si="211"/>
+        <f t="shared" si="226"/>
         <v>25984</v>
       </c>
       <c r="S75" s="1">
-        <f t="shared" si="211"/>
+        <f t="shared" si="226"/>
         <v>31438</v>
       </c>
     </row>
@@ -7280,31 +7283,31 @@
         <v>10949</v>
       </c>
       <c r="M76" s="1">
-        <f t="shared" ref="M76:S76" si="212">+M66+M68</f>
+        <f t="shared" ref="M76:S76" si="227">+M66+M68</f>
         <v>10950</v>
       </c>
       <c r="N76" s="1">
-        <f t="shared" si="212"/>
+        <f t="shared" si="227"/>
         <v>10953</v>
       </c>
       <c r="O76" s="1">
-        <f t="shared" si="212"/>
+        <f t="shared" si="227"/>
         <v>10954</v>
       </c>
       <c r="P76" s="1">
-        <f t="shared" si="212"/>
+        <f t="shared" si="227"/>
         <v>9705</v>
       </c>
       <c r="Q76" s="1">
-        <f t="shared" si="212"/>
+        <f t="shared" si="227"/>
         <v>9706</v>
       </c>
       <c r="R76" s="1">
-        <f t="shared" si="212"/>
+        <f t="shared" si="227"/>
         <v>9709</v>
       </c>
       <c r="S76" s="1">
-        <f t="shared" si="212"/>
+        <f t="shared" si="227"/>
         <v>9710</v>
       </c>
     </row>
@@ -7317,31 +7320,31 @@
         <v>19845</v>
       </c>
       <c r="M77" s="1">
-        <f t="shared" ref="M77:S77" si="213">+M55-M67</f>
+        <f t="shared" ref="M77:S77" si="228">+M55-M67</f>
         <v>16368</v>
       </c>
       <c r="N77" s="1">
-        <f t="shared" si="213"/>
+        <f t="shared" si="228"/>
         <v>16510</v>
       </c>
       <c r="O77" s="1">
-        <f t="shared" si="213"/>
+        <f t="shared" si="228"/>
         <v>17623</v>
       </c>
       <c r="P77" s="1">
-        <f t="shared" si="213"/>
+        <f t="shared" si="228"/>
         <v>18463</v>
       </c>
       <c r="Q77" s="1">
-        <f t="shared" si="213"/>
+        <f t="shared" si="228"/>
         <v>23557</v>
       </c>
       <c r="R77" s="1">
-        <f t="shared" si="213"/>
+        <f t="shared" si="228"/>
         <v>33714</v>
       </c>
       <c r="S77" s="1">
-        <f t="shared" si="213"/>
+        <f t="shared" si="228"/>
         <v>38506</v>
       </c>
     </row>
@@ -7354,31 +7357,31 @@
         <v>3.6204938597649545</v>
       </c>
       <c r="M78" s="22">
-        <f t="shared" ref="M78:S78" si="214">+M55/M67</f>
+        <f t="shared" ref="M78:S78" si="229">+M55/M67</f>
         <v>3.3877461706783372</v>
       </c>
       <c r="N78" s="22">
-        <f t="shared" si="214"/>
+        <f t="shared" si="229"/>
         <v>3.5156178576870332</v>
       </c>
       <c r="O78" s="22">
-        <f t="shared" si="214"/>
+        <f t="shared" si="229"/>
         <v>3.4274104683195592</v>
       </c>
       <c r="P78" s="22">
-        <f t="shared" si="214"/>
+        <f t="shared" si="229"/>
         <v>2.7866266692471453</v>
       </c>
       <c r="Q78" s="22">
-        <f t="shared" si="214"/>
+        <f t="shared" si="229"/>
         <v>3.588396879463795</v>
       </c>
       <c r="R78" s="22">
-        <f t="shared" si="214"/>
+        <f t="shared" si="229"/>
         <v>4.1712915059730973</v>
       </c>
       <c r="S78" s="22">
-        <f t="shared" si="214"/>
+        <f t="shared" si="229"/>
         <v>3.5294619982920579</v>
       </c>
     </row>
@@ -7445,35 +7448,35 @@
         <v>113</v>
       </c>
       <c r="L83" s="4">
-        <f>+SUM(L81:L82)</f>
+        <f t="shared" ref="L83:S83" si="230">+SUM(L81:L82)</f>
         <v>837</v>
       </c>
       <c r="M83" s="4">
-        <f>+SUM(M81:M82)</f>
+        <f t="shared" si="230"/>
         <v>-138</v>
       </c>
       <c r="N83" s="4">
-        <f>+SUM(N81:N82)</f>
+        <f t="shared" si="230"/>
         <v>2758</v>
       </c>
       <c r="O83" s="4">
-        <f>+SUM(O81:O82)</f>
+        <f t="shared" si="230"/>
         <v>2663</v>
       </c>
       <c r="P83" s="4">
-        <f>+SUM(P81:P82)</f>
+        <f t="shared" si="230"/>
         <v>6059</v>
       </c>
       <c r="Q83" s="4">
-        <f>+SUM(Q81:Q82)</f>
+        <f t="shared" si="230"/>
         <v>7055</v>
       </c>
       <c r="R83" s="4">
-        <f>+SUM(R81:R82)</f>
+        <f t="shared" si="230"/>
         <v>11246</v>
       </c>
       <c r="S83" s="4">
-        <f>+SUM(S81:S82)</f>
+        <f t="shared" si="230"/>
         <v>14976</v>
       </c>
       <c r="U83" s="20"/>
@@ -7483,35 +7486,35 @@
         <v>31</v>
       </c>
       <c r="L84" s="1">
-        <f>+L26</f>
+        <f t="shared" ref="L84:S84" si="231">+L26</f>
         <v>656</v>
       </c>
       <c r="M84" s="1">
-        <f>+M26</f>
+        <f t="shared" si="231"/>
         <v>680</v>
       </c>
       <c r="N84" s="1">
-        <f>+N26</f>
+        <f t="shared" si="231"/>
         <v>1414</v>
       </c>
       <c r="O84" s="1">
-        <f>+O26</f>
+        <f t="shared" si="231"/>
         <v>2043</v>
       </c>
       <c r="P84" s="1">
-        <f>+P26</f>
+        <f t="shared" si="231"/>
         <v>6188</v>
       </c>
       <c r="Q84" s="1">
-        <f>+Q26</f>
+        <f t="shared" si="231"/>
         <v>9243</v>
       </c>
       <c r="R84" s="1">
-        <f>+R26</f>
+        <f t="shared" si="231"/>
         <v>12286</v>
       </c>
       <c r="S84" s="1">
-        <f>+S26</f>
+        <f t="shared" si="231"/>
         <v>14881</v>
       </c>
     </row>
@@ -7520,19 +7523,19 @@
         <v>114</v>
       </c>
       <c r="O86" s="1">
-        <f t="shared" ref="O86:R86" si="215">SUM(L83:O83)</f>
+        <f t="shared" ref="O86:R86" si="232">SUM(L83:O83)</f>
         <v>6120</v>
       </c>
       <c r="P86" s="1">
-        <f t="shared" si="215"/>
+        <f t="shared" si="232"/>
         <v>11342</v>
       </c>
       <c r="Q86" s="1">
-        <f t="shared" si="215"/>
+        <f t="shared" si="232"/>
         <v>18535</v>
       </c>
       <c r="R86" s="1">
-        <f t="shared" si="215"/>
+        <f t="shared" si="232"/>
         <v>27023</v>
       </c>
       <c r="S86" s="1">
@@ -7545,19 +7548,19 @@
         <v>115</v>
       </c>
       <c r="O87" s="1">
-        <f t="shared" ref="O87:R87" si="216">SUM(L84:O84)</f>
+        <f t="shared" ref="O87:R87" si="233">SUM(L84:O84)</f>
         <v>4793</v>
       </c>
       <c r="P87" s="1">
-        <f t="shared" si="216"/>
+        <f t="shared" si="233"/>
         <v>10325</v>
       </c>
       <c r="Q87" s="1">
-        <f t="shared" si="216"/>
+        <f t="shared" si="233"/>
         <v>18888</v>
       </c>
       <c r="R87" s="1">
-        <f t="shared" si="216"/>
+        <f t="shared" si="233"/>
         <v>29760</v>
       </c>
       <c r="S87" s="1">

</xml_diff>